<commit_message>
checking relay - problems with initial condition open
</commit_message>
<xml_diff>
--- a/Components/SimulinkOpal/Relay/relay_settings/relay_parameters.xlsx
+++ b/Components/SimulinkOpal/Relay/relay_settings/relay_parameters.xlsx
@@ -187,7 +187,7 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>4</xdr:row>
       <xdr:rowOff>164523</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="6225872" cy="4742452"/>
@@ -732,10 +732,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V9"/>
+  <dimension ref="A1:V7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -852,7 +852,7 @@
         <v>400</v>
       </c>
       <c r="H2" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I2" s="7">
         <v>20</v>
@@ -898,140 +898,18 @@
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A3" s="6">
-        <v>2</v>
-      </c>
-      <c r="B3" s="7">
-        <v>13800</v>
-      </c>
-      <c r="C3" s="8">
-        <v>3</v>
-      </c>
-      <c r="D3" s="8">
-        <v>8</v>
-      </c>
-      <c r="E3" s="8">
-        <v>0.3</v>
-      </c>
-      <c r="F3" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="G3" s="7">
-        <v>250</v>
-      </c>
-      <c r="H3" s="10">
-        <v>1</v>
-      </c>
-      <c r="I3" s="7">
-        <v>20</v>
-      </c>
-      <c r="J3" s="7">
-        <v>0</v>
-      </c>
-      <c r="K3" s="7">
-        <v>0.8</v>
-      </c>
-      <c r="L3" s="7">
-        <v>1</v>
-      </c>
-      <c r="M3" s="7">
-        <v>1</v>
-      </c>
-      <c r="N3" s="7">
-        <v>0.9</v>
-      </c>
-      <c r="O3" s="7">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="P3" s="7">
-        <v>20</v>
-      </c>
-      <c r="Q3" s="7">
-        <v>1</v>
-      </c>
-      <c r="R3" s="7">
-        <v>0.7</v>
-      </c>
-      <c r="S3" s="7">
-        <v>2</v>
-      </c>
-      <c r="T3" s="7">
-        <v>3</v>
-      </c>
-      <c r="U3" s="7">
-        <v>0.9</v>
-      </c>
-      <c r="V3" s="7">
-        <v>1.1000000000000001</v>
-      </c>
+      <c r="A3" s="6"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A4" s="6">
-        <v>3</v>
-      </c>
-      <c r="B4" s="7">
-        <v>13800</v>
-      </c>
-      <c r="C4" s="8">
-        <v>5</v>
-      </c>
-      <c r="D4" s="8">
-        <v>12</v>
-      </c>
-      <c r="E4" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="F4" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="G4" s="7">
-        <v>600</v>
-      </c>
-      <c r="H4" s="10">
-        <v>1</v>
-      </c>
-      <c r="I4" s="7">
-        <v>20</v>
-      </c>
-      <c r="J4" s="7">
-        <v>0</v>
-      </c>
-      <c r="K4" s="7">
-        <v>0.8</v>
-      </c>
-      <c r="L4" s="7">
-        <v>1</v>
-      </c>
-      <c r="M4" s="7">
-        <v>1</v>
-      </c>
-      <c r="N4" s="7">
-        <v>0.9</v>
-      </c>
-      <c r="O4" s="7">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="P4" s="7">
-        <v>20</v>
-      </c>
-      <c r="Q4" s="7">
-        <v>1</v>
-      </c>
-      <c r="R4" s="7">
-        <v>0.7</v>
-      </c>
-      <c r="S4" s="7">
-        <v>2</v>
-      </c>
-      <c r="T4" s="7">
-        <v>3</v>
-      </c>
-      <c r="U4" s="7">
-        <v>0.9</v>
-      </c>
-      <c r="V4" s="7">
-        <v>1.1000000000000001</v>
-      </c>
+      <c r="A4" s="6"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
@@ -1054,20 +932,6 @@
       <c r="E7" s="8"/>
       <c r="F7" s="8"/>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A9" s="6"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
modified method to compute rms - simulink issues
</commit_message>
<xml_diff>
--- a/Components/SimulinkOpal/Relay/relay_settings/relay_parameters.xlsx
+++ b/Components/SimulinkOpal/Relay/relay_settings/relay_parameters.xlsx
@@ -735,7 +735,7 @@
   <dimension ref="A1:V7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -849,7 +849,7 @@
         <v>0.5</v>
       </c>
       <c r="G2" s="7">
-        <v>400</v>
+        <v>1200</v>
       </c>
       <c r="H2" s="10">
         <v>1</v>
@@ -898,11 +898,72 @@
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
+      <c r="A3" s="6">
+        <v>2</v>
+      </c>
+      <c r="B3" s="7">
+        <v>13800</v>
+      </c>
+      <c r="C3" s="8">
+        <v>5</v>
+      </c>
+      <c r="D3" s="8">
+        <v>12</v>
+      </c>
+      <c r="E3" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="F3" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G3" s="7">
+        <v>1200</v>
+      </c>
+      <c r="H3" s="10">
+        <v>1</v>
+      </c>
+      <c r="I3" s="7">
+        <v>20</v>
+      </c>
+      <c r="J3" s="7">
+        <v>0</v>
+      </c>
+      <c r="K3" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="L3" s="7">
+        <v>1</v>
+      </c>
+      <c r="M3" s="7">
+        <v>1</v>
+      </c>
+      <c r="N3" s="7">
+        <v>0.9</v>
+      </c>
+      <c r="O3" s="7">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="P3" s="7">
+        <v>20</v>
+      </c>
+      <c r="Q3" s="7">
+        <v>1</v>
+      </c>
+      <c r="R3" s="7">
+        <v>0.7</v>
+      </c>
+      <c r="S3" s="7">
+        <v>2</v>
+      </c>
+      <c r="T3" s="7">
+        <v>3</v>
+      </c>
+      <c r="U3" s="7">
+        <v>0.9</v>
+      </c>
+      <c r="V3" s="7">
+        <v>1.1000000000000001</v>
+      </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>

</xml_diff>